<commit_message>
Novas atualizações (em 12/01/2021).
</commit_message>
<xml_diff>
--- a/dados/cap4.xlsx
+++ b/dados/cap4.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\glossario_stf\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D98F1D-2F3A-4462-A946-324F9C91FF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFE5D8A-8BFC-451A-A761-BE194499674A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1B3479A7-5E3F-4DCF-999A-B0BE5180553E}"/>
+    <workbookView xWindow="30675" yWindow="1080" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{1B3479A7-5E3F-4DCF-999A-B0BE5180553E}"/>
   </bookViews>
   <sheets>
     <sheet name="acervo_4-1" sheetId="5" r:id="rId1"/>
+    <sheet name="acervo_4-2" sheetId="6" r:id="rId2"/>
+    <sheet name="acervo_4-3" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>Código</t>
   </si>
@@ -52,6 +54,84 @@
   </si>
   <si>
     <t>por prevenção de Turma</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>Autuado</t>
+  </si>
+  <si>
+    <t>TODAS</t>
+  </si>
+  <si>
+    <t>Interposto pedido de extensão</t>
+  </si>
+  <si>
+    <t>Iniciada a execução contra a Fazenda Pública</t>
+  </si>
+  <si>
+    <t>Recebimento externo dos autos</t>
+  </si>
+  <si>
+    <t>Retorno ao trâmite</t>
+  </si>
+  <si>
+    <t>Remessa indevida</t>
+  </si>
+  <si>
+    <t>Remessa externa dos autos, Guia nº</t>
+  </si>
+  <si>
+    <t>Autos restaurados</t>
+  </si>
+  <si>
+    <t>Baixa ao arquivo do STF, Guia nº</t>
+  </si>
+  <si>
+    <t>Baixa definitiva dos autos, Guia nº</t>
+  </si>
+  <si>
+    <t>Cancelamento de autuação</t>
+  </si>
+  <si>
+    <t>Processo findo</t>
+  </si>
+  <si>
+    <t>Reautuado</t>
+  </si>
+  <si>
+    <t>Remessa dos autos ao juízo competente, Guia nº</t>
+  </si>
+  <si>
+    <t>Autos devolvidos à origem</t>
+  </si>
+  <si>
+    <t>Devolução por impossibilidade de processamento</t>
+  </si>
+  <si>
+    <t>Baixa dos autos - distribuição cancelada</t>
+  </si>
+  <si>
+    <t>Processo recebido na origem</t>
+  </si>
+  <si>
+    <t>Comunicado provimento de agravo, Ofício nº</t>
+  </si>
+  <si>
+    <t>Autos entregues ao advogado</t>
+  </si>
+  <si>
+    <t>Apensado ao Processo nº</t>
+  </si>
+  <si>
+    <t>PPE, AI, AC</t>
+  </si>
+  <si>
+    <t>Agravo de Instrumento apensado ao RE nº</t>
+  </si>
+  <si>
+    <t>Retificação de autuação</t>
   </si>
 </sst>
 </file>
@@ -414,7 +494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E262F0C4-1CFA-42B1-86DA-1E3CB60A7526}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -467,4 +547,328 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CBB2B4-6048-48EE-98B3-6A172052C033}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="30.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>7001</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>8001</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>8012</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>8100</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>8101</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D6F5A2-8951-467A-B3CE-73430B52BA4E}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="30.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>7002</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>7101</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>7102</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>7103</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>7104</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>7105</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>7106</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>7106</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>7107</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>7108</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>7109</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>7111</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>7112</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>7113</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>7312</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>8210</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>8233</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>8241</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>8248</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
25/05/2022 - Informações sugeridas atualizadas.
</commit_message>
<xml_diff>
--- a/dados/cap4.xlsx
+++ b/dados/cap4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\glossario_stf\dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arian\Desktop\R_STF\glossario_stf\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFE5D8A-8BFC-451A-A761-BE194499674A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCF2608-749E-489D-BB51-D666485FA6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30675" yWindow="1080" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{1B3479A7-5E3F-4DCF-999A-B0BE5180553E}"/>
+    <workbookView xWindow="23880" yWindow="810" windowWidth="12150" windowHeight="8760" xr2:uid="{1B3479A7-5E3F-4DCF-999A-B0BE5180553E}"/>
   </bookViews>
   <sheets>
     <sheet name="acervo_4-1" sheetId="5" r:id="rId1"/>
@@ -44,18 +44,6 @@
     <t>Andamento</t>
   </si>
   <si>
-    <t>andamentos de distribuição por exclusão</t>
-  </si>
-  <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>por prevenção</t>
-  </si>
-  <si>
-    <t>por prevenção de Turma</t>
-  </si>
-  <si>
     <t>Classes</t>
   </si>
   <si>
@@ -132,6 +120,18 @@
   </si>
   <si>
     <t>Retificação de autuação</t>
+  </si>
+  <si>
+    <t>Distribuído por exclusão de Ministro</t>
+  </si>
+  <si>
+    <t>Distribuído</t>
+  </si>
+  <si>
+    <t>Distribuído por prevenção</t>
+  </si>
+  <si>
+    <t>Distribuído por prevenção de Turma</t>
   </si>
 </sst>
 </file>
@@ -494,16 +494,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E262F0C4-1CFA-42B1-86DA-1E3CB60A7526}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,36 +511,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>7501</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>7502</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>7503</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>7504</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -557,12 +557,12 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -570,62 +570,62 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>7001</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>8001</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>8012</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>8100</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>8101</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -638,16 +638,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D6F5A2-8951-467A-B3CE-73430B52BA4E}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -655,216 +655,216 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>7002</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>7101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>7102</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>7103</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>7104</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>7105</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7106</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7106</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7107</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7108</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7109</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>7111</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>7112</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>7113</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>7312</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>8210</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>8233</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>8241</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>8248</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>